<commit_message>
add bpsk I/Q display
</commit_message>
<xml_diff>
--- a/2400_iir_llpf_calc.xlsx
+++ b/2400_iir_llpf_calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3EAC70-FF8E-CE44-A48A-E1FB4F95186A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF064781-42C1-B240-A300-D1EB8204F820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15000" yWindow="140" windowWidth="13800" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,7 +250,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -302,7 +302,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -507,7 +507,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -551,7 +551,7 @@
       </c>
       <c r="B4">
         <f>2*PI()*B2</f>
-        <v>628.31853071795865</v>
+        <v>314.15926535897933</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -578,7 +578,7 @@
       </c>
       <c r="B6">
         <f>(2*B3)*TAN(B4*B5/2)</f>
-        <v>628.4182355179048</v>
+        <v>314.17172667928406</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -593,7 +593,7 @@
       </c>
       <c r="B8">
         <f>B6*B5</f>
-        <v>4.3640155244298942E-2</v>
+        <v>2.1817481019394725E-2</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
@@ -605,7 +605,7 @@
       </c>
       <c r="B9">
         <f>2+(B8)</f>
-        <v>2.0436401552442991</v>
+        <v>2.0218174810193945</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -614,7 +614,7 @@
       </c>
       <c r="B10">
         <f>2-B8</f>
-        <v>1.9563598447557011</v>
+        <v>1.9781825189806053</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -623,7 +623,7 @@
       </c>
       <c r="B12">
         <f>B10/B9</f>
-        <v>0.95729174225480784</v>
+        <v>0.97841795194253212</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -635,7 +635,7 @@
       </c>
       <c r="B13">
         <f>B8/B9</f>
-        <v>2.1354128872596041E-2</v>
+        <v>1.0791024028733996E-2</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -647,7 +647,7 @@
       </c>
       <c r="B14">
         <f>B8/B9</f>
-        <v>2.1354128872596041E-2</v>
+        <v>1.0791024028733996E-2</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -658,7 +658,7 @@
         <v>25</v>
       </c>
       <c r="B16" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -684,7 +684,7 @@
       </c>
       <c r="B20" s="1">
         <f>ROUND(B19*B13*B16,0)</f>
-        <v>5598</v>
+        <v>1414</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
@@ -696,7 +696,7 @@
       </c>
       <c r="B21" s="1">
         <f>ROUND(B19*B14*B16,0)</f>
-        <v>5598</v>
+        <v>1414</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
@@ -708,7 +708,7 @@
       </c>
       <c r="B22" s="1">
         <f>ROUND(B19*B12,0)</f>
-        <v>31369</v>
+        <v>32061</v>
       </c>
       <c r="D22" t="s">
         <v>20</v>
@@ -727,7 +727,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -968,7 +968,7 @@
       </c>
       <c r="B1">
         <f>'LoopFilter LPF'!B16</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -994,7 +994,7 @@
       </c>
       <c r="B4">
         <f>B3*B2*B1</f>
-        <v>0.48</v>
+        <v>0.24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tuning qpsk 2400 and 4800
</commit_message>
<xml_diff>
--- a/2400_iir_llpf_calc.xlsx
+++ b/2400_iir_llpf_calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="15000" yWindow="135" windowWidth="13800" windowHeight="17865"/>
+    <workbookView xWindow="15000" yWindow="135" windowWidth="13800" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="LoopFilter LPF" sheetId="4" r:id="rId1"/>
@@ -490,7 +490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -533,7 +533,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>14400</v>
+        <v>7200</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -557,7 +557,7 @@
       </c>
       <c r="B5">
         <f>1/B3</f>
-        <v>6.9444444444444444E-5</v>
+        <v>1.3888888888888889E-4</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -572,7 +572,7 @@
       </c>
       <c r="B6">
         <f>(2*B3)*TAN(B4*B5/2)</f>
-        <v>1257.4351557651473</v>
+        <v>1259.8367547733058</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -587,7 +587,7 @@
       </c>
       <c r="B8">
         <f>B6*B5</f>
-        <v>8.7321885817024117E-2</v>
+        <v>0.17497732705184801</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
@@ -599,7 +599,7 @@
       </c>
       <c r="B9">
         <f>2+(B8)</f>
-        <v>2.0873218858170239</v>
+        <v>2.174977327051848</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -608,7 +608,7 @@
       </c>
       <c r="B10">
         <f>2-B8</f>
-        <v>1.9126781141829758</v>
+        <v>1.825022672948152</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -617,7 +617,7 @@
       </c>
       <c r="B12">
         <f>B10/B9</f>
-        <v>0.91633117401742348</v>
+        <v>0.83909963117728004</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -629,7 +629,7 @@
       </c>
       <c r="B13">
         <f>B8/B9</f>
-        <v>4.183441299128831E-2</v>
+        <v>8.0450184411359996E-2</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -641,7 +641,7 @@
       </c>
       <c r="B14">
         <f>B8/B9</f>
-        <v>4.183441299128831E-2</v>
+        <v>8.0450184411359996E-2</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -678,7 +678,7 @@
       </c>
       <c r="B20" s="1">
         <f>ROUND(B19*B13*B16,0)</f>
-        <v>1371</v>
+        <v>2636</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
@@ -690,7 +690,7 @@
       </c>
       <c r="B21" s="1">
         <f>ROUND(B19*B14*B16,0)</f>
-        <v>1371</v>
+        <v>2636</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
@@ -702,7 +702,7 @@
       </c>
       <c r="B22" s="1">
         <f>ROUND(B19*B12,0)</f>
-        <v>30026</v>
+        <v>27496</v>
       </c>
       <c r="D22" t="s">
         <v>20</v>
@@ -713,6 +713,7 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -720,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -753,7 +754,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>14400</v>
+        <v>7200</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -777,7 +778,7 @@
       </c>
       <c r="B5">
         <f>1/B3</f>
-        <v>6.9444444444444444E-5</v>
+        <v>1.3888888888888889E-4</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -792,7 +793,7 @@
       </c>
       <c r="B6">
         <f>(2*B3)*TAN(B4*B5/2)</f>
-        <v>7716.9367420163335</v>
+        <v>8313.8438763306112</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -807,7 +808,7 @@
       </c>
       <c r="B8">
         <f>B6*B5</f>
-        <v>0.53589838486224539</v>
+        <v>1.1547005383792515</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
@@ -819,7 +820,7 @@
       </c>
       <c r="B9">
         <f>2+(B8)</f>
-        <v>2.5358983848622456</v>
+        <v>3.1547005383792515</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -828,7 +829,7 @@
       </c>
       <c r="B10">
         <f>2-B8</f>
-        <v>1.4641016151377546</v>
+        <v>0.84529946162074854</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -837,7 +838,7 @@
       </c>
       <c r="B12">
         <f>B10/B9</f>
-        <v>0.57735026918962573</v>
+        <v>0.26794919243112275</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -849,7 +850,7 @@
       </c>
       <c r="B13">
         <f>B8/B9</f>
-        <v>0.21132486540518708</v>
+        <v>0.36602540378443865</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -861,7 +862,7 @@
       </c>
       <c r="B14">
         <f>B8/B9</f>
-        <v>0.21132486540518708</v>
+        <v>0.36602540378443865</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -878,7 +879,7 @@
         <v>25</v>
       </c>
       <c r="B18" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -904,7 +905,7 @@
       </c>
       <c r="B22" s="1">
         <f>ROUND(B21*B13*B18,0)</f>
-        <v>27699</v>
+        <v>23988</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
@@ -916,7 +917,7 @@
       </c>
       <c r="B23" s="1">
         <f>ROUND(B21*B14*B18,0)</f>
-        <v>27699</v>
+        <v>23988</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
@@ -928,7 +929,7 @@
       </c>
       <c r="B24" s="1">
         <f>ROUND(B21*B12,0)</f>
-        <v>18919</v>
+        <v>8780</v>
       </c>
       <c r="D24" t="s">
         <v>20</v>
@@ -940,6 +941,7 @@
     <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -971,7 +973,7 @@
       </c>
       <c r="B2">
         <f>'Branch LPF'!B18</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -988,7 +990,7 @@
       </c>
       <c r="B4">
         <f>B3*B2*B1</f>
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>